<commit_message>
minor changes to download file name and about tab in file
</commit_message>
<xml_diff>
--- a/shiny/readme.xlsx
+++ b/shiny/readme.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clam\Desktop\travel-study-stories\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clam\Desktop\travel-study-stories\shiny\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9989E97D-5E56-4F3E-B2B3-28064E6596FB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A0690B-0A5C-477F-8078-1D917D91D0BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1780" windowWidth="16920" windowHeight="10540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Data Source: [2017 Puget Sound Regional Household Travel Survey] (https://www.psrc.org/household-travel-survey-program) </t>
-  </si>
   <si>
     <t>How Are Survey Results Used?</t>
   </si>
@@ -50,6 +47,9 @@
   </si>
   <si>
     <t>About</t>
+  </si>
+  <si>
+    <t>Data Source: [2017/19 Puget Sound Regional Household Travel Survey] (https://www.psrc.org/household-travel-survey-program) </t>
   </si>
 </sst>
 </file>
@@ -892,58 +892,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>